<commit_message>
data for batch fermentation modified, more data points added
</commit_message>
<xml_diff>
--- a/Data/Batch_fermentation_data.xlsx
+++ b/Data/Batch_fermentation_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claud\Documents\dyn-pam\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C2C06D-9A09-4E8F-8C98-E808A6110072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE08E666-30EA-4B85-AF37-DC2E0684DF3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>EX_glc__D_e</t>
   </si>
@@ -64,13 +64,7 @@
     <t>EX_ac_e</t>
   </si>
   <si>
-    <t>BIOMASS_Ecoli_core_w_GAM</t>
-  </si>
-  <si>
     <t>t [1/h]</t>
-  </si>
-  <si>
-    <t>all metabolites concentration in mmol/L</t>
   </si>
   <si>
     <t>biomass [mg]</t>
@@ -81,24 +75,27 @@
   <si>
     <t>c_biomass [g/L]</t>
   </si>
+  <si>
+    <t>BIOMASS_Ec_iML1515_core_75p37M</t>
+  </si>
+  <si>
+    <t>metabolites concentration in mmol/L</t>
+  </si>
+  <si>
+    <t>biomass concentration in g/L</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -417,15 +414,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DCCE7C9-4CE9-4D14-8D64-25E93447D220}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -435,10 +439,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,7 +455,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -460,16 +464,16 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -590,7 +594,7 @@
         <v>15</v>
       </c>
       <c r="F10">
-        <f t="shared" ref="F7:F12" si="0">D10/E10</f>
+        <f t="shared" ref="F10:F27" si="0">D10/E10</f>
         <v>0.5493333333333339</v>
       </c>
       <c r="G10">
@@ -643,6 +647,310 @@
       </c>
       <c r="G12">
         <v>1.0320000000000011</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5.5</v>
+      </c>
+      <c r="B13">
+        <v>72.224953255494015</v>
+      </c>
+      <c r="C13">
+        <v>5.6399241327975016</v>
+      </c>
+      <c r="E13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>66.275143181334016</v>
+      </c>
+      <c r="C14">
+        <v>7.0607167421733008</v>
+      </c>
+      <c r="D14">
+        <v>23.839999999999918</v>
+      </c>
+      <c r="E14">
+        <v>15</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>1.5893333333333279</v>
+      </c>
+      <c r="G14">
+        <v>1.5893333333333279</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>6.5</v>
+      </c>
+      <c r="B15">
+        <v>58.480370071020012</v>
+      </c>
+      <c r="C15">
+        <v>8.6985527400000002</v>
+      </c>
+      <c r="D15">
+        <v>33.679999999999836</v>
+      </c>
+      <c r="E15">
+        <v>15</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>2.2453333333333223</v>
+      </c>
+      <c r="G15">
+        <v>2.2453333333333223</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>7</v>
+      </c>
+      <c r="B16">
+        <v>47.992959960039002</v>
+      </c>
+      <c r="C16">
+        <v>11.148210167463002</v>
+      </c>
+      <c r="D16">
+        <v>43.029999999999973</v>
+      </c>
+      <c r="E16">
+        <v>15</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>2.8686666666666647</v>
+      </c>
+      <c r="G16">
+        <v>2.8686666666666647</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>7.5</v>
+      </c>
+      <c r="B17">
+        <v>33.998641326399607</v>
+      </c>
+      <c r="C17">
+        <v>15.568524718173004</v>
+      </c>
+      <c r="D17">
+        <v>53.009999999999991</v>
+      </c>
+      <c r="E17">
+        <v>15</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>3.5339999999999994</v>
+      </c>
+      <c r="G17">
+        <v>3.5339999999999994</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>9.2437780257432021</v>
+      </c>
+      <c r="C18">
+        <v>11.493629696768402</v>
+      </c>
+      <c r="D18">
+        <v>76.309999999999945</v>
+      </c>
+      <c r="E18">
+        <v>15</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>5.0873333333333299</v>
+      </c>
+      <c r="G18">
+        <v>5.0873333333333299</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>8.5</v>
+      </c>
+      <c r="B19">
+        <v>0.18628907533511402</v>
+      </c>
+      <c r="C19">
+        <v>10.302101942443201</v>
+      </c>
+      <c r="D19">
+        <v>90.330000000000155</v>
+      </c>
+      <c r="E19">
+        <v>15</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>6.02200000000001</v>
+      </c>
+      <c r="G19">
+        <v>6.02200000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>9</v>
+      </c>
+      <c r="B20">
+        <v>0.20577774782144703</v>
+      </c>
+      <c r="C20">
+        <v>2.1002365638972007</v>
+      </c>
+      <c r="E20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>9.5</v>
+      </c>
+      <c r="B21">
+        <v>0.17025155364837602</v>
+      </c>
+      <c r="C21">
+        <v>5.6758346580258009E-2</v>
+      </c>
+      <c r="E21">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>10</v>
+      </c>
+      <c r="B22">
+        <v>0.19101586889403005</v>
+      </c>
+      <c r="C22">
+        <v>3.7647626210478007E-2</v>
+      </c>
+      <c r="D22">
+        <v>88.479999999999791</v>
+      </c>
+      <c r="E22">
+        <v>15</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>5.898666666666653</v>
+      </c>
+      <c r="G22">
+        <v>5.898666666666653</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>10.5</v>
+      </c>
+      <c r="B23">
+        <v>0.19088147625419705</v>
+      </c>
+      <c r="C23">
+        <v>3.4205608891260009E-2</v>
+      </c>
+      <c r="E23">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>11</v>
+      </c>
+      <c r="B24">
+        <v>0.22064748880284002</v>
+      </c>
+      <c r="C24">
+        <v>3.8400775901883004E-2</v>
+      </c>
+      <c r="E24">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>11.5</v>
+      </c>
+      <c r="B25">
+        <v>0.24528787914943803</v>
+      </c>
+      <c r="C25">
+        <v>3.4070346396153008E-2</v>
+      </c>
+      <c r="D25">
+        <v>87.410000000000082</v>
+      </c>
+      <c r="E25">
+        <v>15</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>5.827333333333339</v>
+      </c>
+      <c r="G25">
+        <v>5.827333333333339</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>12</v>
+      </c>
+      <c r="B26">
+        <v>0.26730435106201506</v>
+      </c>
+      <c r="C26">
+        <v>3.6958120929954E-2</v>
+      </c>
+      <c r="E26">
+        <v>5</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>12.5</v>
+      </c>
+      <c r="B27">
+        <v>0.27065111922873003</v>
+      </c>
+      <c r="C27">
+        <v>3.8127496369968011E-2</v>
+      </c>
+      <c r="D27">
+        <v>82.369999999999891</v>
+      </c>
+      <c r="E27">
+        <v>15</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>5.4913333333333263</v>
+      </c>
+      <c r="G27">
+        <v>5.4913333333333263</v>
       </c>
     </row>
   </sheetData>
@@ -653,17 +961,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA2B006-A395-4AA2-89C2-BA28CFE10784}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -672,7 +980,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -806,6 +1114,198 @@
       </c>
       <c r="D12">
         <v>1.0320000000000011</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5.5</v>
+      </c>
+      <c r="B13">
+        <v>72.224953255494015</v>
+      </c>
+      <c r="C13">
+        <v>5.6399241327975016</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>66.275143181334016</v>
+      </c>
+      <c r="C14">
+        <v>7.0607167421733008</v>
+      </c>
+      <c r="D14">
+        <v>1.5893333333333279</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>6.5</v>
+      </c>
+      <c r="B15">
+        <v>58.480370071020012</v>
+      </c>
+      <c r="C15">
+        <v>8.6985527400000002</v>
+      </c>
+      <c r="D15">
+        <v>2.2453333333333223</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>7</v>
+      </c>
+      <c r="B16">
+        <v>47.992959960039002</v>
+      </c>
+      <c r="C16">
+        <v>11.148210167463002</v>
+      </c>
+      <c r="D16">
+        <v>2.8686666666666647</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>7.5</v>
+      </c>
+      <c r="B17">
+        <v>33.998641326399607</v>
+      </c>
+      <c r="C17">
+        <v>15.568524718173004</v>
+      </c>
+      <c r="D17">
+        <v>3.5339999999999994</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>9.2437780257432021</v>
+      </c>
+      <c r="C18">
+        <v>11.493629696768402</v>
+      </c>
+      <c r="D18">
+        <v>5.0873333333333299</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>8.5</v>
+      </c>
+      <c r="B19">
+        <v>0.18628907533511402</v>
+      </c>
+      <c r="C19">
+        <v>10.302101942443201</v>
+      </c>
+      <c r="D19">
+        <v>6.02200000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>9</v>
+      </c>
+      <c r="B20">
+        <v>0.20577774782144703</v>
+      </c>
+      <c r="C20">
+        <v>2.1002365638972007</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>9.5</v>
+      </c>
+      <c r="B21">
+        <v>0.17025155364837602</v>
+      </c>
+      <c r="C21">
+        <v>5.6758346580258009E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>10</v>
+      </c>
+      <c r="B22">
+        <v>0.19101586889403005</v>
+      </c>
+      <c r="C22">
+        <v>3.7647626210478007E-2</v>
+      </c>
+      <c r="D22">
+        <v>5.898666666666653</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>10.5</v>
+      </c>
+      <c r="B23">
+        <v>0.19088147625419705</v>
+      </c>
+      <c r="C23">
+        <v>3.4205608891260009E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>11</v>
+      </c>
+      <c r="B24">
+        <v>0.22064748880284002</v>
+      </c>
+      <c r="C24">
+        <v>3.8400775901883004E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>11.5</v>
+      </c>
+      <c r="B25">
+        <v>0.24528787914943803</v>
+      </c>
+      <c r="C25">
+        <v>3.4070346396153008E-2</v>
+      </c>
+      <c r="D25">
+        <v>5.827333333333339</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>12</v>
+      </c>
+      <c r="B26">
+        <v>0.26730435106201506</v>
+      </c>
+      <c r="C26">
+        <v>3.6958120929954E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>12.5</v>
+      </c>
+      <c r="B27">
+        <v>0.27065111922873003</v>
+      </c>
+      <c r="C27">
+        <v>3.8127496369968011E-2</v>
+      </c>
+      <c r="D27">
+        <v>5.4913333333333263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tried simulation with different solver
</commit_message>
<xml_diff>
--- a/Data/Batch_fermentation_data.xlsx
+++ b/Data/Batch_fermentation_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claud\Documents\dyn-pam\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE08E666-30EA-4B85-AF37-DC2E0684DF3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D9184B-22A9-40E9-B996-64318DB1F790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -441,7 +441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
@@ -963,7 +963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA2B006-A395-4AA2-89C2-BA28CFE10784}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
simulation run with different km and vmax value, solver tolerance issue found
</commit_message>
<xml_diff>
--- a/Data/Batch_fermentation_data.xlsx
+++ b/Data/Batch_fermentation_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claud\Documents\dyn-pam\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\claud\PycharmProjects\PythonProject\DFBA_PAM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D9184B-22A9-40E9-B996-64318DB1F790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FACFCA0-EC59-4C9B-B2C6-744186087928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="75" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -29,8 +29,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -45,10 +43,19 @@
   <commentList>
     <comment ref="G1" authorId="0" shapeId="0" xr:uid="{05E4347C-8FD3-4AA4-854C-4508D7DC2D56}">
       <text>
-        <t>[Kommentarthread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
     C_biomass / DW_biomass (DW_biomass=1g/mmol)</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -122,7 +129,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -420,7 +427,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -442,10 +449,10 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.7109375" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
@@ -955,7 +962,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -964,10 +972,10 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>